<commit_message>
update default image extension
</commit_message>
<xml_diff>
--- a/runs/details-runs.xlsx
+++ b/runs/details-runs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\Workspace\MorphoClassification\runs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348AF5C5-91F4-4C9B-971C-29B06BEC3EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081A5B5D-229E-42DC-AE4F-B6D57FA71827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{C65F539B-C0A9-49E1-9A5E-F53BB71A818B}"/>
+    <workbookView xWindow="-83" yWindow="428" windowWidth="23191" windowHeight="13335" xr2:uid="{C65F539B-C0A9-49E1-9A5E-F53BB71A818B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Run</t>
   </si>
@@ -113,6 +113,21 @@
   </si>
   <si>
     <t>drop rate</t>
+  </si>
+  <si>
+    <t>batch size</t>
+  </si>
+  <si>
+    <t>create_transform((3,320,224))</t>
+  </si>
+  <si>
+    <t>strict_full_balanced</t>
+  </si>
+  <si>
+    <t>mobilenetv2_120d_001</t>
+  </si>
+  <si>
+    <t>mobilenetv2_120d</t>
   </si>
 </sst>
 </file>
@@ -166,7 +181,25 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -331,21 +364,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D963D837-857C-4C2A-9AD1-C8FFEC974342}" name="Table1" displayName="Table1" ref="A1:L30" totalsRowShown="0" dataDxfId="2">
-  <autoFilter ref="A1:L30" xr:uid="{D963D837-857C-4C2A-9AD1-C8FFEC974342}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{A2A4AC59-4E08-487D-8128-2E5227D003D3}" name="Run" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{69A1E7F0-4024-4652-9847-223C3997802D}" name="model name" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{A176CBFA-B9A5-4213-A1DB-C0A5403F61E0}" name="split" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{1E7ECB8C-6A3D-4882-8BEE-E482399A90C0}" name="train folds" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{201D33CA-1383-41EC-A9DD-AB0CC5B9E6B1}" name="val folds" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{3D79EE30-351B-404A-B882-05CEC669E07D}" name="test folds" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{1183B551-65FB-4C4C-91C8-B7AC7ED99F4A}" name="num classes" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{46B69E6A-B43A-4291-BBE2-15EC6DFE04C1}" name="drop rate" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{AC6CE929-D023-4E66-AE0A-4CBE42737E74}" name="in channels" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{0E050D88-8452-43DB-A78A-328B05D4387D}" name="Dataset" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{80F0E4DC-DC2B-4427-9B91-6F24091F3A24}" name="transform" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{E549229C-E545-4C0F-A6DE-27BE447E67DA}" name="image dir" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D963D837-857C-4C2A-9AD1-C8FFEC974342}" name="Table1" displayName="Table1" ref="A1:M30" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A1:M30" xr:uid="{D963D837-857C-4C2A-9AD1-C8FFEC974342}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{A2A4AC59-4E08-487D-8128-2E5227D003D3}" name="Run" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{69A1E7F0-4024-4652-9847-223C3997802D}" name="model name" dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{D92EEBE1-A852-4684-80C1-165F9425D75F}" name="batch size" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{A176CBFA-B9A5-4213-A1DB-C0A5403F61E0}" name="split" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{1E7ECB8C-6A3D-4882-8BEE-E482399A90C0}" name="train folds" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{201D33CA-1383-41EC-A9DD-AB0CC5B9E6B1}" name="val folds" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{3D79EE30-351B-404A-B882-05CEC669E07D}" name="test folds" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{1183B551-65FB-4C4C-91C8-B7AC7ED99F4A}" name="num classes" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{46B69E6A-B43A-4291-BBE2-15EC6DFE04C1}" name="drop rate" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{AC6CE929-D023-4E66-AE0A-4CBE42737E74}" name="in channels" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{0E050D88-8452-43DB-A78A-328B05D4387D}" name="Dataset" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{80F0E4DC-DC2B-4427-9B91-6F24091F3A24}" name="transform" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{E549229C-E545-4C0F-A6DE-27BE447E67DA}" name="image dir" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -668,28 +702,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FEBC23-407C-49A1-99CF-20466B1750B9}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="43.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -697,117 +733,204 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>8</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>9</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>5</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>0</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>3</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>3</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>3</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1">
+        <v>32</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="1">
+        <v>8</v>
+      </c>
+      <c r="G5" s="1">
+        <v>9</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>3</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -820,8 +943,9 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -834,8 +958,9 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -848,8 +973,9 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -862,8 +988,9 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -876,8 +1003,9 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -890,8 +1018,9 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -904,8 +1033,9 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -918,8 +1048,9 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -932,8 +1063,9 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -946,8 +1078,9 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -960,8 +1093,9 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -974,8 +1108,9 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -988,8 +1123,9 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1002,8 +1138,9 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1016,8 +1153,9 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1030,8 +1168,9 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1044,8 +1183,9 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1058,8 +1198,9 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1072,8 +1213,9 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1086,8 +1228,9 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1100,8 +1243,9 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26" s="1"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1114,8 +1258,9 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1128,8 +1273,9 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28" s="1"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1142,8 +1288,9 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1156,6 +1303,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add log train acc, remove save best loss model
</commit_message>
<xml_diff>
--- a/runs/details-runs.xlsx
+++ b/runs/details-runs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\Workspace\MorphoClassification\runs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081A5B5D-229E-42DC-AE4F-B6D57FA71827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE02609-ED6B-4D50-A935-4A042C20EACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="428" windowWidth="23191" windowHeight="13335" xr2:uid="{C65F539B-C0A9-49E1-9A5E-F53BB71A818B}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{C65F539B-C0A9-49E1-9A5E-F53BB71A818B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t>Run</t>
   </si>
@@ -128,6 +128,18 @@
   </si>
   <si>
     <t>mobilenetv2_120d</t>
+  </si>
+  <si>
+    <t>resnet50_002</t>
+  </si>
+  <si>
+    <t>resnet50_003</t>
+  </si>
+  <si>
+    <t>resnet50_004</t>
+  </si>
+  <si>
+    <t>num_epoch_unfreeze</t>
   </si>
 </sst>
 </file>
@@ -181,7 +193,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
     <dxf>
       <font>
         <b val="0"/>
@@ -198,6 +210,50 @@
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
       </font>
     </dxf>
     <dxf>
@@ -275,46 +331,20 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
     </dxf>
     <dxf>
@@ -364,22 +394,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D963D837-857C-4C2A-9AD1-C8FFEC974342}" name="Table1" displayName="Table1" ref="A1:M30" totalsRowShown="0" dataDxfId="3">
-  <autoFilter ref="A1:M30" xr:uid="{D963D837-857C-4C2A-9AD1-C8FFEC974342}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D963D837-857C-4C2A-9AD1-C8FFEC974342}" name="Table1" displayName="Table1" ref="A1:N30" totalsRowShown="0" dataDxfId="14">
+  <autoFilter ref="A1:N30" xr:uid="{D963D837-857C-4C2A-9AD1-C8FFEC974342}"/>
+  <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{A2A4AC59-4E08-487D-8128-2E5227D003D3}" name="Run" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{69A1E7F0-4024-4652-9847-223C3997802D}" name="model name" dataDxfId="12"/>
-    <tableColumn id="14" xr3:uid="{D92EEBE1-A852-4684-80C1-165F9425D75F}" name="batch size" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{A176CBFA-B9A5-4213-A1DB-C0A5403F61E0}" name="split" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{1E7ECB8C-6A3D-4882-8BEE-E482399A90C0}" name="train folds" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{201D33CA-1383-41EC-A9DD-AB0CC5B9E6B1}" name="val folds" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{3D79EE30-351B-404A-B882-05CEC669E07D}" name="test folds" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{1183B551-65FB-4C4C-91C8-B7AC7ED99F4A}" name="num classes" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{46B69E6A-B43A-4291-BBE2-15EC6DFE04C1}" name="drop rate" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{AC6CE929-D023-4E66-AE0A-4CBE42737E74}" name="in channels" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{0E050D88-8452-43DB-A78A-328B05D4387D}" name="Dataset" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{80F0E4DC-DC2B-4427-9B91-6F24091F3A24}" name="transform" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{E549229C-E545-4C0F-A6DE-27BE447E67DA}" name="image dir" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{D92EEBE1-A852-4684-80C1-165F9425D75F}" name="batch size" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{A176CBFA-B9A5-4213-A1DB-C0A5403F61E0}" name="split" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{1E7ECB8C-6A3D-4882-8BEE-E482399A90C0}" name="train folds" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{201D33CA-1383-41EC-A9DD-AB0CC5B9E6B1}" name="val folds" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{3D79EE30-351B-404A-B882-05CEC669E07D}" name="test folds" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{1183B551-65FB-4C4C-91C8-B7AC7ED99F4A}" name="num classes" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{46B69E6A-B43A-4291-BBE2-15EC6DFE04C1}" name="drop rate" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{AC6CE929-D023-4E66-AE0A-4CBE42737E74}" name="in channels" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{0E050D88-8452-43DB-A78A-328B05D4387D}" name="Dataset" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{80F0E4DC-DC2B-4427-9B91-6F24091F3A24}" name="transform" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{0A1CD093-4338-4E90-AC8B-23CFD2CCCA58}" name="num_epoch_unfreeze" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{E549229C-E545-4C0F-A6DE-27BE447E67DA}" name="image dir" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -702,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FEBC23-407C-49A1-99CF-20466B1750B9}">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,7 +756,7 @@
     <col min="13" max="13" width="43.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -763,10 +794,13 @@
         <v>14</v>
       </c>
       <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -803,13 +837,14 @@
       <c r="L2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="1"/>
+      <c r="N2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
@@ -844,13 +879,14 @@
       <c r="L3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="1"/>
+      <c r="N3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>12</v>
@@ -885,11 +921,12 @@
       <c r="L4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="1"/>
+      <c r="N4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -926,26 +963,56 @@
       <c r="L5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="1"/>
+      <c r="N5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1">
+        <v>8</v>
+      </c>
+      <c r="G6" s="1">
+        <v>9</v>
+      </c>
+      <c r="H6" s="1">
+        <v>5</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>3</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="1">
+        <v>10</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -959,8 +1026,9 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -974,8 +1042,9 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -989,8 +1058,9 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1004,8 +1074,9 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1019,8 +1090,9 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1034,8 +1106,9 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1049,8 +1122,9 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1064,8 +1138,9 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1079,8 +1154,9 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1094,8 +1170,9 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1109,8 +1186,9 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1124,8 +1202,9 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1139,8 +1218,9 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="1"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1154,8 +1234,9 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1169,8 +1250,9 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1184,8 +1266,9 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22" s="1"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1199,8 +1282,9 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1214,8 +1298,9 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1229,8 +1314,9 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1244,8 +1330,9 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1259,8 +1346,9 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27" s="1"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1274,8 +1362,9 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" s="1"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1289,8 +1378,9 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" s="1"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1304,6 +1394,7 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>